<commit_message>
Developoing Nominal Range Sens
</commit_message>
<xml_diff>
--- a/R/Dose Response/SummaryComparison 12.xlsx
+++ b/R/Dose Response/SummaryComparison 12.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Share Table QMRA\Share-Table-QMRA\R\Dose Response\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5170E799-E9E4-4374-979B-CB5BA81EA963}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FAF14F-057D-4918-BEFC-79F5DBA22041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SummaryComparison" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SummaryComparison!$A$12:$Y$12</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="52">
   <si>
     <t>Treatment</t>
   </si>
@@ -120,16 +133,73 @@
   </si>
   <si>
     <t>Exposed Students</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>ONWash</t>
+  </si>
+  <si>
+    <t>ONWr</t>
+  </si>
+  <si>
+    <t>OFFWash</t>
+  </si>
+  <si>
+    <t>OFFWr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.136% [0.34%-2.20%]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.129% [0.40%-2.10%]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.173% [0.39%-2.18%]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.656% [0.14%-1.34%]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.071% [0.33%-2.07%]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.675% [0.0%-1.49%]  </t>
+  </si>
+  <si>
+    <t>Intervention Illness Effectiveness (means)</t>
+  </si>
+  <si>
+    <t>Top 2.5th percentile</t>
+  </si>
+  <si>
+    <t>Bottom 2.5th Percentile</t>
+  </si>
+  <si>
+    <t>ST OFF,  Wrapp ON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST OFF, Wash ON </t>
+  </si>
+  <si>
+    <t>ST ON,  Wrapp ON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST ON, Wash ON </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,8 +341,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -452,8 +535,20 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4F8F9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -577,6 +672,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFD6DADC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFD6DADC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -622,7 +728,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -633,7 +739,7 @@
     <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -641,9 +747,6 @@
     </xf>
     <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -663,11 +766,20 @@
     <xf numFmtId="10" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1023,14 +1135,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T29"/>
+  <dimension ref="A1:Y33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E8"/>
+      <selection activeCell="B11" sqref="B11:V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1042,100 +1154,101 @@
     <col min="5" max="5" width="9.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="1" customWidth="1"/>
     <col min="7" max="11" width="9.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="1.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="1.28515625" style="1" customWidth="1"/>
     <col min="13" max="16" width="9.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="0.85546875" style="11" customWidth="1"/>
-    <col min="18" max="18" width="16.140625" style="11" customWidth="1"/>
+    <col min="17" max="17" width="1.140625" style="10" customWidth="1"/>
+    <col min="18" max="18" width="16.140625" style="10" customWidth="1"/>
     <col min="19" max="19" width="18.28515625" style="1" customWidth="1"/>
     <col min="20" max="20" width="11.5703125" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="1"/>
+    <col min="21" max="22" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="7" t="s">
+    <row r="1" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="7" t="s">
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="R1" s="7" t="s">
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="R1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="7"/>
-    </row>
-    <row r="2" spans="1:20" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="S1" s="15"/>
+    </row>
+    <row r="2" spans="1:22" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="12"/>
-      <c r="M2" s="10" t="s">
+      <c r="L2" s="11"/>
+      <c r="M2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="10" t="s">
+      <c r="P2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="10" t="s">
+      <c r="Q2" s="11"/>
+      <c r="R2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="S2" s="10" t="s">
+      <c r="S2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="T2" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1169,7 +1282,7 @@
       <c r="K3" s="5">
         <v>0.22800000000000001</v>
       </c>
-      <c r="L3" s="13"/>
+      <c r="L3" s="12"/>
       <c r="M3" s="4">
         <v>0.82099296523103404</v>
       </c>
@@ -1182,8 +1295,8 @@
       <c r="P3" s="4">
         <v>6.7513538134521003E-2</v>
       </c>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14">
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13">
         <f>SUM(N3:P3)</f>
         <v>0.17900703476896601</v>
       </c>
@@ -1194,7 +1307,7 @@
         <v>1.054</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1228,7 +1341,7 @@
       <c r="K4" s="5">
         <v>0.41099999999999998</v>
       </c>
-      <c r="L4" s="13"/>
+      <c r="L4" s="12"/>
       <c r="M4" s="4">
         <v>0.84747533372025496</v>
       </c>
@@ -1241,8 +1354,8 @@
       <c r="P4" s="4">
         <v>5.8386535113174702E-2</v>
       </c>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14">
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13">
         <f>SUM(N4:P4)</f>
         <v>0.15252466627974462</v>
       </c>
@@ -1253,7 +1366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1287,7 +1400,7 @@
       <c r="K5" s="5">
         <v>0.224</v>
       </c>
-      <c r="L5" s="13"/>
+      <c r="L5" s="12"/>
       <c r="M5" s="4">
         <v>0.82229702572347307</v>
       </c>
@@ -1300,8 +1413,8 @@
       <c r="P5" s="4">
         <v>6.3153135048231501E-2</v>
       </c>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14">
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13">
         <f t="shared" ref="R5:R8" si="0">SUM(N5:P5)</f>
         <v>0.17770297427652729</v>
       </c>
@@ -1312,7 +1425,7 @@
         <v>1.018</v>
       </c>
     </row>
-    <row r="6" spans="1:20" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -1346,7 +1459,7 @@
       <c r="K6" s="5">
         <v>0.224</v>
       </c>
-      <c r="L6" s="13"/>
+      <c r="L6" s="12"/>
       <c r="M6" s="4">
         <v>0.85645884784033099</v>
       </c>
@@ -1359,8 +1472,8 @@
       <c r="P6" s="4">
         <v>3.92117332795726E-2</v>
       </c>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14">
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13">
         <f t="shared" si="0"/>
         <v>0.14354115215966939</v>
       </c>
@@ -1371,7 +1484,7 @@
         <v>0.622</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -1405,7 +1518,7 @@
       <c r="K7" s="5">
         <v>0.41099999999999998</v>
       </c>
-      <c r="L7" s="13"/>
+      <c r="L7" s="12"/>
       <c r="M7" s="4">
         <v>0.8440631118277091</v>
       </c>
@@ -1418,8 +1531,8 @@
       <c r="P7" s="4">
         <v>6.1844984452378203E-2</v>
       </c>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14">
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13">
         <f t="shared" si="0"/>
         <v>0.15593688817229071</v>
       </c>
@@ -1430,7 +1543,7 @@
         <v>0.97299999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:20" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -1464,7 +1577,7 @@
       <c r="K8" s="5">
         <v>0.41199999999999998</v>
       </c>
-      <c r="L8" s="13"/>
+      <c r="L8" s="12"/>
       <c r="M8" s="4">
         <v>0.87608404633024806</v>
       </c>
@@ -1477,8 +1590,8 @@
       <c r="P8" s="4">
         <v>3.6086374483441E-2</v>
       </c>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14">
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13">
         <f t="shared" si="0"/>
         <v>0.1239159536697514</v>
       </c>
@@ -1489,59 +1602,1168 @@
         <v>0.60299999999999998</v>
       </c>
     </row>
-    <row r="24" spans="13:18" x14ac:dyDescent="0.2">
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="15"/>
-    </row>
-    <row r="25" spans="13:18" x14ac:dyDescent="0.2">
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
-      <c r="P25" s="6"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="15"/>
-    </row>
-    <row r="26" spans="13:18" x14ac:dyDescent="0.2">
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
-      <c r="P26" s="6"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
-    </row>
-    <row r="27" spans="13:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="R11" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+    </row>
+    <row r="12" spans="1:22" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L12" s="11"/>
+      <c r="M12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="S12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T12" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="U12" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="V12" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="2">
+        <v>100</v>
+      </c>
+      <c r="D13" s="3">
+        <v>162500</v>
+      </c>
+      <c r="E13" s="3">
+        <v>57468</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0.3536492</v>
+      </c>
+      <c r="G13" s="3">
+        <v>98050</v>
+      </c>
+      <c r="H13" s="3">
+        <v>57468</v>
+      </c>
+      <c r="I13" s="3">
+        <v>40582</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0.58610909999999994</v>
+      </c>
+      <c r="K13" s="5">
+        <v>0.41389090000000001</v>
+      </c>
+      <c r="L13" s="12"/>
+      <c r="M13" s="4">
+        <v>0.84036330000000004</v>
+      </c>
+      <c r="N13" s="4">
+        <v>6.5740930000000003E-2</v>
+      </c>
+      <c r="O13" s="4">
+        <v>3.4854179999999998E-2</v>
+      </c>
+      <c r="P13" s="4">
+        <v>5.9041550000000005E-2</v>
+      </c>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13">
+        <f>SUM(N13:P13)</f>
+        <v>0.15963666000000001</v>
+      </c>
+      <c r="S13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="T13" s="4">
+        <v>1</v>
+      </c>
+      <c r="U13" s="4">
+        <v>1</v>
+      </c>
+      <c r="V13" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="2">
+        <v>100</v>
+      </c>
+      <c r="D14" s="3">
+        <v>162500</v>
+      </c>
+      <c r="E14" s="3">
+        <v>57587</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0.35438150000000002</v>
+      </c>
+      <c r="G14" s="3">
+        <v>97827</v>
+      </c>
+      <c r="H14" s="3">
+        <v>57587</v>
+      </c>
+      <c r="I14" s="3">
+        <v>40240</v>
+      </c>
+      <c r="J14" s="4">
+        <v>0.58866160000000001</v>
+      </c>
+      <c r="K14" s="5">
+        <v>0.41133839999999999</v>
+      </c>
+      <c r="L14" s="12"/>
+      <c r="M14" s="4">
+        <v>0.84645840000000006</v>
+      </c>
+      <c r="N14" s="4">
+        <v>6.3295539999999997E-2</v>
+      </c>
+      <c r="O14" s="4">
+        <v>3.4104920000000004E-2</v>
+      </c>
+      <c r="P14" s="4">
+        <v>5.6141139999999999E-2</v>
+      </c>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13">
+        <f>SUM(N14:P14)</f>
+        <v>0.1535416</v>
+      </c>
+      <c r="S14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="T14" s="4">
+        <v>0.94335561456596306</v>
+      </c>
+      <c r="U14" s="4">
+        <v>0.94231515936299215</v>
+      </c>
+      <c r="V14" s="4">
+        <v>0.97401870858040418</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>3</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="2">
+        <v>100</v>
+      </c>
+      <c r="D15" s="3">
+        <v>162500</v>
+      </c>
+      <c r="E15" s="3">
+        <v>57407</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.35327379999999997</v>
+      </c>
+      <c r="G15" s="3">
+        <v>98013</v>
+      </c>
+      <c r="H15" s="3">
+        <v>57407</v>
+      </c>
+      <c r="I15" s="3">
+        <v>40606</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0.58570800000000001</v>
+      </c>
+      <c r="K15" s="5">
+        <v>0.41429199999999999</v>
+      </c>
+      <c r="L15" s="12"/>
+      <c r="M15" s="4">
+        <v>0.8767919999999999</v>
+      </c>
+      <c r="N15" s="4">
+        <v>6.3232709999999998E-2</v>
+      </c>
+      <c r="O15" s="4">
+        <v>2.4596300000000001E-2</v>
+      </c>
+      <c r="P15" s="4">
+        <v>3.5378960000000001E-2</v>
+      </c>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13">
+        <f>SUM(N15:P15)</f>
+        <v>0.12320797</v>
+      </c>
+      <c r="S15" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="T15" s="4">
+        <v>0.58635564045321353</v>
+      </c>
+      <c r="U15" s="4">
+        <v>0.67631871420409573</v>
+      </c>
+      <c r="V15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>4</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="2">
+        <v>100</v>
+      </c>
+      <c r="D16" s="3">
+        <v>162500</v>
+      </c>
+      <c r="E16" s="3">
+        <v>65941</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.40579079999999995</v>
+      </c>
+      <c r="G16" s="3">
+        <v>91095</v>
+      </c>
+      <c r="H16" s="3">
+        <v>70664</v>
+      </c>
+      <c r="I16" s="3">
+        <v>20431</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0.77571769999999995</v>
+      </c>
+      <c r="K16" s="5">
+        <v>0.22428229999999999</v>
+      </c>
+      <c r="L16" s="12"/>
+      <c r="M16" s="4">
+        <v>0.8150771</v>
+      </c>
+      <c r="N16" s="4">
+        <v>7.8858370000000011E-2</v>
+      </c>
+      <c r="O16" s="4">
+        <v>3.8913570000000001E-2</v>
+      </c>
+      <c r="P16" s="4">
+        <v>6.7150939999999992E-2</v>
+      </c>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13">
+        <f>SUM(N16:P16)</f>
+        <v>0.18492288000000001</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="T16" s="4">
+        <v>1.0327111822883308</v>
+      </c>
+      <c r="U16" s="4">
+        <v>0.99069289498448443</v>
+      </c>
+      <c r="V16" s="4">
+        <v>1.1749659105642232</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>5</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="2">
+        <v>100</v>
+      </c>
+      <c r="D17" s="3">
+        <v>162500</v>
+      </c>
+      <c r="E17" s="3">
+        <v>66238</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.40761850000000005</v>
+      </c>
+      <c r="G17" s="3">
+        <v>91199</v>
+      </c>
+      <c r="H17" s="3">
+        <v>70925</v>
+      </c>
+      <c r="I17" s="3">
+        <v>20274</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0.77769490000000008</v>
+      </c>
+      <c r="K17" s="5">
+        <v>0.22230509999999998</v>
+      </c>
+      <c r="L17" s="12"/>
+      <c r="M17" s="4">
+        <v>0.82072220000000007</v>
+      </c>
+      <c r="N17" s="4">
+        <v>7.8429299999999993E-2</v>
+      </c>
+      <c r="O17" s="4">
+        <v>3.6897249999999999E-2</v>
+      </c>
+      <c r="P17" s="4">
+        <v>6.3951209999999994E-2</v>
+      </c>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13">
+        <f>SUM(N17:P17)</f>
+        <v>0.17927776000000001</v>
+      </c>
+      <c r="S17" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="T17" s="4">
+        <v>0.99333869980140765</v>
+      </c>
+      <c r="U17" s="4">
+        <v>0.97930797945387027</v>
+      </c>
+      <c r="V17" s="4">
+        <v>1.2165295389618034</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="2">
+        <v>100</v>
+      </c>
+      <c r="D18" s="3">
+        <v>162500</v>
+      </c>
+      <c r="E18" s="3">
+        <v>65721</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0.40443689999999999</v>
+      </c>
+      <c r="G18" s="3">
+        <v>90809</v>
+      </c>
+      <c r="H18" s="3">
+        <v>70153</v>
+      </c>
+      <c r="I18" s="3">
+        <v>20656</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0.77253360000000004</v>
+      </c>
+      <c r="K18" s="5">
+        <v>0.22746639999999999</v>
+      </c>
+      <c r="L18" s="12"/>
+      <c r="M18" s="4">
+        <v>0.86576589999999998</v>
+      </c>
+      <c r="N18" s="4">
+        <v>6.9886340000000005E-2</v>
+      </c>
+      <c r="O18" s="4">
+        <v>2.7388509999999998E-2</v>
+      </c>
+      <c r="P18" s="4">
+        <v>3.6959270000000002E-2</v>
+      </c>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13">
+        <f>SUM(N18:P18)</f>
+        <v>0.13423412000000001</v>
+      </c>
+      <c r="S18" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="T18" s="4">
+        <v>0.57718468580714766</v>
+      </c>
+      <c r="U18" s="4">
+        <v>0.6058978828171051</v>
+      </c>
+      <c r="V18" s="4">
+        <v>0.41802217191805424</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="17">
+        <v>1</v>
+      </c>
+      <c r="B21" s="16">
+        <v>1</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="16">
+        <v>100</v>
+      </c>
+      <c r="E21" s="16">
+        <v>162500</v>
+      </c>
+      <c r="F21" s="16">
+        <v>65941</v>
+      </c>
+      <c r="G21" s="16">
+        <v>40.579079999999998</v>
+      </c>
+      <c r="H21" s="16">
+        <v>91095</v>
+      </c>
+      <c r="I21" s="16">
+        <v>70664</v>
+      </c>
+      <c r="J21" s="16">
+        <v>20431</v>
+      </c>
+      <c r="K21" s="16">
+        <v>77.571770000000001</v>
+      </c>
+      <c r="L21" s="16">
+        <v>22.428229999999999</v>
+      </c>
+      <c r="M21" s="16">
+        <v>81.507710000000003</v>
+      </c>
+      <c r="N21" s="16">
+        <v>7.8858370000000004</v>
+      </c>
+      <c r="O21" s="16">
+        <v>3.8913570000000002</v>
+      </c>
+      <c r="P21" s="16">
+        <v>6.7150939999999997</v>
+      </c>
+      <c r="Q21" s="16">
+        <v>1.1728441000000001</v>
+      </c>
+      <c r="R21" s="16">
+        <v>2.1865890000000001</v>
+      </c>
+      <c r="S21" s="16">
+        <v>0.39421810000000002</v>
+      </c>
+      <c r="T21" s="1">
+        <v>1.0327111822883308</v>
+      </c>
+      <c r="U21" s="1">
+        <f>R21/$R$22</f>
+        <v>0.99069289498448443</v>
+      </c>
+      <c r="V21" s="1">
+        <f>S21/$S$22</f>
+        <v>1.1749659105642232</v>
+      </c>
+      <c r="W21" s="1">
+        <v>100</v>
+      </c>
+      <c r="X21" s="1">
+        <v>100</v>
+      </c>
+      <c r="Y21" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="17">
+        <v>2</v>
+      </c>
+      <c r="B22" s="16">
+        <v>2</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="16">
+        <v>100</v>
+      </c>
+      <c r="E22" s="16">
+        <v>162500</v>
+      </c>
+      <c r="F22" s="16">
+        <v>57468</v>
+      </c>
+      <c r="G22" s="16">
+        <v>35.364919999999998</v>
+      </c>
+      <c r="H22" s="16">
+        <v>98050</v>
+      </c>
+      <c r="I22" s="16">
+        <v>57468</v>
+      </c>
+      <c r="J22" s="16">
+        <v>40582</v>
+      </c>
+      <c r="K22" s="16">
+        <v>58.610909999999997</v>
+      </c>
+      <c r="L22" s="16">
+        <v>41.389090000000003</v>
+      </c>
+      <c r="M22" s="16">
+        <v>84.036330000000007</v>
+      </c>
+      <c r="N22" s="16">
+        <v>6.5740930000000004</v>
+      </c>
+      <c r="O22" s="16">
+        <v>3.4854180000000001</v>
+      </c>
+      <c r="P22" s="16">
+        <v>5.9041550000000003</v>
+      </c>
+      <c r="Q22" s="16">
+        <v>1.1356942000000001</v>
+      </c>
+      <c r="R22" s="16">
+        <v>2.207131</v>
+      </c>
+      <c r="S22" s="16">
+        <v>0.33551449999999999</v>
+      </c>
+      <c r="T22" s="1">
+        <v>1</v>
+      </c>
+      <c r="U22" s="1">
+        <f t="shared" ref="U22:U26" si="1">R22/$R$22</f>
+        <v>1</v>
+      </c>
+      <c r="V22" s="1">
+        <f t="shared" ref="V22:V26" si="2">S22/$S$22</f>
+        <v>1</v>
+      </c>
+      <c r="W22" s="1">
+        <v>100</v>
+      </c>
+      <c r="X22" s="1">
+        <v>100</v>
+      </c>
+      <c r="Y22" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="17">
+        <v>3</v>
+      </c>
+      <c r="B23" s="16">
+        <v>3</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="16">
+        <v>100</v>
+      </c>
+      <c r="E23" s="16">
+        <v>162500</v>
+      </c>
+      <c r="F23" s="16">
+        <v>66238</v>
+      </c>
+      <c r="G23" s="16">
+        <v>40.761850000000003</v>
+      </c>
+      <c r="H23" s="16">
+        <v>91199</v>
+      </c>
+      <c r="I23" s="16">
+        <v>70925</v>
+      </c>
+      <c r="J23" s="16">
+        <v>20274</v>
+      </c>
+      <c r="K23" s="16">
+        <v>77.769490000000005</v>
+      </c>
+      <c r="L23" s="16">
+        <v>22.230509999999999</v>
+      </c>
+      <c r="M23" s="16">
+        <v>82.072220000000002</v>
+      </c>
+      <c r="N23" s="16">
+        <v>7.84293</v>
+      </c>
+      <c r="O23" s="16">
+        <v>3.6897250000000001</v>
+      </c>
+      <c r="P23" s="16">
+        <v>6.3951209999999996</v>
+      </c>
+      <c r="Q23" s="16">
+        <v>1.1281289999999999</v>
+      </c>
+      <c r="R23" s="16">
+        <v>2.1614610000000001</v>
+      </c>
+      <c r="S23" s="16">
+        <v>0.40816330000000001</v>
+      </c>
+      <c r="T23" s="1">
+        <v>0.99333869980140765</v>
+      </c>
+      <c r="U23" s="1">
+        <f t="shared" si="1"/>
+        <v>0.97930797945387027</v>
+      </c>
+      <c r="V23" s="1">
+        <f t="shared" si="2"/>
+        <v>1.2165295389618034</v>
+      </c>
+      <c r="W23" s="1">
+        <v>100</v>
+      </c>
+      <c r="X23" s="1">
+        <v>100</v>
+      </c>
+      <c r="Y23" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="17">
+        <v>4</v>
+      </c>
+      <c r="B24" s="16">
+        <v>4</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="16">
+        <v>100</v>
+      </c>
+      <c r="E24" s="16">
+        <v>162500</v>
+      </c>
+      <c r="F24" s="16">
+        <v>65721</v>
+      </c>
+      <c r="G24" s="16">
+        <v>40.443689999999997</v>
+      </c>
+      <c r="H24" s="16">
+        <v>90809</v>
+      </c>
+      <c r="I24" s="16">
+        <v>70153</v>
+      </c>
+      <c r="J24" s="16">
+        <v>20656</v>
+      </c>
+      <c r="K24" s="16">
+        <v>77.253360000000001</v>
+      </c>
+      <c r="L24" s="16">
+        <v>22.746639999999999</v>
+      </c>
+      <c r="M24" s="16">
+        <v>86.576589999999996</v>
+      </c>
+      <c r="N24" s="16">
+        <v>6.9886340000000002</v>
+      </c>
+      <c r="O24" s="16">
+        <v>2.7388509999999999</v>
+      </c>
+      <c r="P24" s="16">
+        <v>3.6959270000000002</v>
+      </c>
+      <c r="Q24" s="16">
+        <v>0.65550529999999996</v>
+      </c>
+      <c r="R24" s="16">
+        <v>1.337296</v>
+      </c>
+      <c r="S24" s="16">
+        <v>0.1402525</v>
+      </c>
+      <c r="T24" s="1">
+        <v>0.57718468580714766</v>
+      </c>
+      <c r="U24" s="1">
+        <f t="shared" si="1"/>
+        <v>0.6058978828171051</v>
+      </c>
+      <c r="V24" s="1">
+        <f t="shared" si="2"/>
+        <v>0.41802217191805424</v>
+      </c>
+      <c r="W24" s="1">
+        <v>100</v>
+      </c>
+      <c r="X24" s="1">
+        <v>100</v>
+      </c>
+      <c r="Y24" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="17">
+        <v>5</v>
+      </c>
+      <c r="B25" s="16">
+        <v>5</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="16">
+        <v>100</v>
+      </c>
+      <c r="E25" s="16">
+        <v>162500</v>
+      </c>
+      <c r="F25" s="16">
+        <v>57587</v>
+      </c>
+      <c r="G25" s="16">
+        <v>35.43815</v>
+      </c>
+      <c r="H25" s="16">
+        <v>97827</v>
+      </c>
+      <c r="I25" s="16">
+        <v>57587</v>
+      </c>
+      <c r="J25" s="16">
+        <v>40240</v>
+      </c>
+      <c r="K25" s="16">
+        <v>58.866160000000001</v>
+      </c>
+      <c r="L25" s="16">
+        <v>41.133839999999999</v>
+      </c>
+      <c r="M25" s="16">
+        <v>84.645840000000007</v>
+      </c>
+      <c r="N25" s="16">
+        <v>6.3295539999999999</v>
+      </c>
+      <c r="O25" s="16">
+        <v>3.4104920000000001</v>
+      </c>
+      <c r="P25" s="16">
+        <v>5.6141139999999998</v>
+      </c>
+      <c r="Q25" s="16">
+        <v>1.0713634999999999</v>
+      </c>
+      <c r="R25" s="16">
+        <v>2.0798130000000001</v>
+      </c>
+      <c r="S25" s="16">
+        <v>0.32679740000000002</v>
+      </c>
+      <c r="T25" s="1">
+        <v>0.94335561456596306</v>
+      </c>
+      <c r="U25" s="1">
+        <f t="shared" si="1"/>
+        <v>0.94231515936299215</v>
+      </c>
+      <c r="V25" s="1">
+        <f t="shared" si="2"/>
+        <v>0.97401870858040418</v>
+      </c>
+      <c r="W25" s="1">
+        <v>100</v>
+      </c>
+      <c r="X25" s="1">
+        <v>100</v>
+      </c>
+      <c r="Y25" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="17">
+        <v>6</v>
+      </c>
+      <c r="B26" s="16">
+        <v>6</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="16">
+        <v>100</v>
+      </c>
+      <c r="E26" s="16">
+        <v>162500</v>
+      </c>
+      <c r="F26" s="16">
+        <v>57407</v>
+      </c>
+      <c r="G26" s="16">
+        <v>35.327379999999998</v>
+      </c>
+      <c r="H26" s="16">
+        <v>98013</v>
+      </c>
+      <c r="I26" s="16">
+        <v>57407</v>
+      </c>
+      <c r="J26" s="16">
+        <v>40606</v>
+      </c>
+      <c r="K26" s="16">
+        <v>58.570799999999998</v>
+      </c>
+      <c r="L26" s="16">
+        <v>41.429200000000002</v>
+      </c>
+      <c r="M26" s="16">
+        <v>87.679199999999994</v>
+      </c>
+      <c r="N26" s="16">
+        <v>6.3232710000000001</v>
+      </c>
+      <c r="O26" s="16">
+        <v>2.4596300000000002</v>
+      </c>
+      <c r="P26" s="16">
+        <v>3.5378959999999999</v>
+      </c>
+      <c r="Q26" s="16">
+        <v>0.66592070000000003</v>
+      </c>
+      <c r="R26" s="16">
+        <v>1.4927239999999999</v>
+      </c>
+      <c r="S26" s="16">
+        <v>0</v>
+      </c>
+      <c r="T26" s="1">
+        <v>0.58635564045321353</v>
+      </c>
+      <c r="U26" s="1">
+        <f t="shared" si="1"/>
+        <v>0.67631871420409573</v>
+      </c>
+      <c r="V26" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W26" s="1">
+        <v>100</v>
+      </c>
+      <c r="X26" s="1">
+        <v>100</v>
+      </c>
+      <c r="Y26" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="M27" s="6"/>
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
-    </row>
-    <row r="28" spans="13:18" x14ac:dyDescent="0.2">
-      <c r="M28" s="6"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="6"/>
-      <c r="P28" s="6"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
-    </row>
-    <row r="29" spans="13:18" x14ac:dyDescent="0.2">
-      <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="6"/>
-      <c r="P29" s="6"/>
-      <c r="Q29" s="15"/>
-      <c r="R29" s="15"/>
+      <c r="Q27" s="14"/>
+      <c r="R27" s="14"/>
+    </row>
+    <row r="28" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G28" s="1">
+        <f>G21/W21</f>
+        <v>0.40579079999999995</v>
+      </c>
+      <c r="K28" s="16">
+        <f>K21/W21</f>
+        <v>0.77571769999999995</v>
+      </c>
+      <c r="L28" s="1">
+        <f>L21/W21</f>
+        <v>0.22428229999999999</v>
+      </c>
+      <c r="M28" s="6">
+        <f>M21/W21</f>
+        <v>0.8150771</v>
+      </c>
+      <c r="N28" s="6">
+        <f>N21/W21</f>
+        <v>7.8858370000000011E-2</v>
+      </c>
+      <c r="O28" s="6">
+        <f>O21/X21</f>
+        <v>3.8913570000000001E-2</v>
+      </c>
+      <c r="P28" s="6">
+        <f>P21/Y21</f>
+        <v>6.7150939999999992E-2</v>
+      </c>
+      <c r="Q28" s="14"/>
+      <c r="R28" s="14"/>
+    </row>
+    <row r="29" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G29" s="1">
+        <f>G22/W22</f>
+        <v>0.3536492</v>
+      </c>
+      <c r="K29" s="16">
+        <f>K22/W22</f>
+        <v>0.58610909999999994</v>
+      </c>
+      <c r="L29" s="1">
+        <f>L22/W22</f>
+        <v>0.41389090000000001</v>
+      </c>
+      <c r="M29" s="6">
+        <f>M22/W22</f>
+        <v>0.84036330000000004</v>
+      </c>
+      <c r="N29" s="6">
+        <f>N22/W22</f>
+        <v>6.5740930000000003E-2</v>
+      </c>
+      <c r="O29" s="6">
+        <f>O22/X22</f>
+        <v>3.4854179999999998E-2</v>
+      </c>
+      <c r="P29" s="6">
+        <f>P22/Y22</f>
+        <v>5.9041550000000005E-2</v>
+      </c>
+      <c r="Q29" s="14"/>
+      <c r="R29" s="14"/>
+    </row>
+    <row r="30" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G30" s="1">
+        <f>G23/W23</f>
+        <v>0.40761850000000005</v>
+      </c>
+      <c r="K30" s="16">
+        <f>K23/W23</f>
+        <v>0.77769490000000008</v>
+      </c>
+      <c r="L30" s="1">
+        <f>L23/W23</f>
+        <v>0.22230509999999998</v>
+      </c>
+      <c r="M30" s="6">
+        <f>M23/W23</f>
+        <v>0.82072220000000007</v>
+      </c>
+      <c r="N30" s="6">
+        <f>N23/W23</f>
+        <v>7.8429299999999993E-2</v>
+      </c>
+      <c r="O30" s="6">
+        <f>O23/X23</f>
+        <v>3.6897249999999999E-2</v>
+      </c>
+      <c r="P30" s="6">
+        <f>P23/Y23</f>
+        <v>6.3951209999999994E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G31" s="1">
+        <f>G24/W24</f>
+        <v>0.40443689999999999</v>
+      </c>
+      <c r="K31" s="16">
+        <f>K24/W24</f>
+        <v>0.77253360000000004</v>
+      </c>
+      <c r="L31" s="1">
+        <f>L24/W24</f>
+        <v>0.22746639999999999</v>
+      </c>
+      <c r="M31" s="6">
+        <f>M24/W24</f>
+        <v>0.86576589999999998</v>
+      </c>
+      <c r="N31" s="6">
+        <f>N24/W24</f>
+        <v>6.9886340000000005E-2</v>
+      </c>
+      <c r="O31" s="6">
+        <f>O24/X24</f>
+        <v>2.7388509999999998E-2</v>
+      </c>
+      <c r="P31" s="6">
+        <f>P24/Y24</f>
+        <v>3.6959270000000002E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G32" s="1">
+        <f>G25/W25</f>
+        <v>0.35438150000000002</v>
+      </c>
+      <c r="K32" s="16">
+        <f>K25/W25</f>
+        <v>0.58866160000000001</v>
+      </c>
+      <c r="L32" s="1">
+        <f>L25/W25</f>
+        <v>0.41133839999999999</v>
+      </c>
+      <c r="M32" s="6">
+        <f>M25/W25</f>
+        <v>0.84645840000000006</v>
+      </c>
+      <c r="N32" s="6">
+        <f>N25/W25</f>
+        <v>6.3295539999999997E-2</v>
+      </c>
+      <c r="O32" s="6">
+        <f>O25/X25</f>
+        <v>3.4104920000000004E-2</v>
+      </c>
+      <c r="P32" s="6">
+        <f>P25/Y25</f>
+        <v>5.6141139999999999E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="7:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G33" s="1">
+        <f>G26/W26</f>
+        <v>0.35327379999999997</v>
+      </c>
+      <c r="K33" s="16">
+        <f>K26/W26</f>
+        <v>0.58570800000000001</v>
+      </c>
+      <c r="L33" s="1">
+        <f>L26/W26</f>
+        <v>0.41429199999999999</v>
+      </c>
+      <c r="M33" s="6">
+        <f>M26/W26</f>
+        <v>0.8767919999999999</v>
+      </c>
+      <c r="N33" s="6">
+        <f>N26/W26</f>
+        <v>6.3232709999999998E-2</v>
+      </c>
+      <c r="O33" s="6">
+        <f>O26/X26</f>
+        <v>2.4596300000000001E-2</v>
+      </c>
+      <c r="P33" s="6">
+        <f>P26/Y26</f>
+        <v>3.5378960000000001E-2</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <autoFilter ref="A12:Y12" xr:uid="{30BA0471-5028-47C3-A6EB-F4ABB78D3DBA}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A13:Y18">
+      <sortCondition ref="A12"/>
+    </sortState>
+  </autoFilter>
+  <mergeCells count="6">
     <mergeCell ref="M1:P1"/>
     <mergeCell ref="H1:K1"/>
     <mergeCell ref="R1:S1"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="M11:P11"/>
+    <mergeCell ref="R11:V11"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
updates to food waste
</commit_message>
<xml_diff>
--- a/R/Dose Response/SummaryComparison 12.xlsx
+++ b/R/Dose Response/SummaryComparison 12.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Share Table QMRA\Share-Table-QMRA\R\Dose Response\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E0669A-5C60-4002-85BE-533CA3508822}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19770638-3C78-420E-9C9F-A0E204895C6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SummaryComparison" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,12 @@
     <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
     <sheet name="3-3-21" sheetId="6" r:id="rId6"/>
     <sheet name="3-8-21" sheetId="7" r:id="rId7"/>
+    <sheet name="3-9-21 " sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'3-3-21'!$A$1:$S$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'3-8-21'!$A$1:$S$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'3-9-21 '!$A$1:$S$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet2!$A$1:$R$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sheet4!$A$1:$S$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SummaryComparison!$A$4:$Y$4</definedName>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="105">
   <si>
     <t>Treatment</t>
   </si>
@@ -339,6 +341,27 @@
   <si>
     <t xml:space="preserve">0.99% [0.28%-1.97%]  </t>
   </si>
+  <si>
+    <t xml:space="preserve">0.89% [0.17%-1.81%]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.48% [0.0%-1.21%]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.98% [0.28%-2.07%]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.90% [0.28%-1.97%]  </t>
+  </si>
+  <si>
+    <t>0.86% [0.17%-1.80%]</t>
+  </si>
+  <si>
+    <t>0.93% [0.27%-1.96%]</t>
+  </si>
+  <si>
+    <t>0.92% [0.27%-1.89%]</t>
+  </si>
 </sst>
 </file>
 
@@ -509,7 +532,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -701,6 +724,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -882,7 +911,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -953,6 +982,10 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1344,26 +1377,26 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
       <c r="L3" s="10"/>
-      <c r="M3" s="23" t="s">
+      <c r="M3" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="R3" s="23" t="s">
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="R3" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="S3" s="23"/>
-      <c r="T3" s="23"/>
-      <c r="U3" s="23"/>
-      <c r="V3" s="23"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="24"/>
+      <c r="U3" s="24"/>
+      <c r="V3" s="24"/>
     </row>
     <row r="4" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
@@ -7733,7 +7766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04AEF58A-6676-4911-9A0F-F93CCACAFA8C}">
   <dimension ref="A1:AP20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AM2" sqref="AM2:AP7"/>
     </sheetView>
   </sheetViews>
@@ -7745,7 +7778,7 @@
     <col min="39" max="39" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="77.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7866,7 +7899,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:42" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -8142,7 +8175,7 @@
         <v>0.98566308243727407</v>
       </c>
     </row>
-    <row r="4" spans="1:42" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6</v>
       </c>
@@ -8272,7 +8305,7 @@
         <v>0.58992862383292344</v>
       </c>
       <c r="AO4" s="4">
-        <f t="shared" ref="AO3:AO9" si="8">S14</f>
+        <f t="shared" ref="AO4:AO9" si="8">S14</f>
         <v>0</v>
       </c>
       <c r="AP4" s="4">
@@ -8280,7 +8313,7 @@
         <v>0.66956521739130581</v>
       </c>
     </row>
-    <row r="5" spans="1:42" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -8418,7 +8451,7 @@
         <v>1.1395337118886808</v>
       </c>
     </row>
-    <row r="6" spans="1:42" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -8556,7 +8589,7 @@
         <v>1.1047345767575303</v>
       </c>
     </row>
-    <row r="7" spans="1:42" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -8694,7 +8727,7 @@
         <v>0.64421669106881285</v>
       </c>
     </row>
-    <row r="8" spans="1:42" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9</v>
       </c>
@@ -8832,7 +8865,7 @@
         <v>0.99458731381459897</v>
       </c>
     </row>
-    <row r="9" spans="1:42" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -8970,7 +9003,7 @@
         <v>1.0784691857107456</v>
       </c>
     </row>
-    <row r="10" spans="1:42" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -9139,7 +9172,7 @@
         <v>4.6023901048612696E-2</v>
       </c>
       <c r="P12">
-        <f>P2/$P$2</f>
+        <f t="shared" ref="P12:P20" si="23">P2/$P$2</f>
         <v>1</v>
       </c>
       <c r="R12">
@@ -9153,291 +9186,291 @@
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="F13">
-        <f t="shared" ref="F13:F20" si="23">F3/$A$12</f>
+        <f t="shared" ref="F13:F20" si="24">F3/$A$12</f>
         <v>0.35374769230769204</v>
       </c>
       <c r="J13">
-        <f t="shared" ref="J13:O20" si="24">J3/$A$12</f>
+        <f t="shared" ref="J13:O20" si="25">J3/$A$12</f>
         <v>0.62186883029073703</v>
       </c>
       <c r="K13">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.37813116970926303</v>
       </c>
       <c r="L13">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.85597731542690103</v>
       </c>
       <c r="M13">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>6.78188713381115E-2</v>
       </c>
       <c r="N13">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>3.0625913297613199E-2</v>
       </c>
       <c r="O13">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>4.5577899937373899E-2</v>
       </c>
       <c r="P13">
-        <f>P3/$P$2</f>
+        <f t="shared" si="23"/>
         <v>0.99654063698340667</v>
       </c>
       <c r="R13">
-        <f t="shared" ref="R13:R20" si="25">R3/$R$2</f>
+        <f t="shared" ref="R13:R20" si="26">R3/$R$2</f>
         <v>0.98566308243727407</v>
       </c>
       <c r="S13">
-        <f t="shared" ref="S13:S18" si="26">S3/$S$2</f>
+        <f t="shared" ref="S13:S18" si="27">S3/$S$2</f>
         <v>0.9966101694915287</v>
       </c>
     </row>
     <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="F14">
+        <f t="shared" si="24"/>
+        <v>0.35273230769230801</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="25"/>
+        <v>0.62117583310755897</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="25"/>
+        <v>0.37882416689244103</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="25"/>
+        <v>0.88959158394249693</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="25"/>
+        <v>6.16200561768349E-2</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="25"/>
+        <v>2.1493745529405597E-2</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="25"/>
+        <v>2.7294614351262202E-2</v>
+      </c>
+      <c r="P14">
         <f t="shared" si="23"/>
-        <v>0.35273230769230801</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="24"/>
-        <v>0.62117583310755897</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="24"/>
-        <v>0.37882416689244103</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="24"/>
-        <v>0.88959158394249693</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="24"/>
-        <v>6.16200561768349E-2</v>
-      </c>
-      <c r="N14">
-        <f t="shared" si="24"/>
-        <v>2.1493745529405597E-2</v>
-      </c>
-      <c r="O14">
-        <f t="shared" si="24"/>
-        <v>2.7294614351262202E-2</v>
-      </c>
-      <c r="P14">
-        <f>P4/$P$2</f>
         <v>0.58992862383292344</v>
       </c>
       <c r="R14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.66956521739130581</v>
       </c>
       <c r="S14">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="F15">
+        <f t="shared" si="24"/>
+        <v>0.40807384615384601</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="25"/>
+        <v>0.82812591047350492</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="25"/>
+        <v>0.17187408952649499</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="25"/>
+        <v>0.79053564965617096</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="25"/>
+        <v>0.10250784171793899</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="25"/>
+        <v>4.5557365182772293E-2</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="25"/>
+        <v>6.13991434431174E-2</v>
+      </c>
+      <c r="P15">
         <f t="shared" si="23"/>
-        <v>0.40807384615384601</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="24"/>
-        <v>0.82812591047350492</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="24"/>
-        <v>0.17187408952649499</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="24"/>
-        <v>0.79053564965617096</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="24"/>
-        <v>0.10250784171793899</v>
-      </c>
-      <c r="N15">
-        <f t="shared" si="24"/>
-        <v>4.5557365182772293E-2</v>
-      </c>
-      <c r="O15">
-        <f t="shared" si="24"/>
-        <v>6.13991434431174E-2</v>
-      </c>
-      <c r="P15">
-        <f>P5/$P$2</f>
         <v>1.2215042525828173</v>
       </c>
       <c r="R15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1.1395337118886808</v>
       </c>
       <c r="S15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1.6220689655172436</v>
       </c>
     </row>
     <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="F16">
+        <f t="shared" si="24"/>
+        <v>0.40683076923076894</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="25"/>
+        <v>0.82905707849389998</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="25"/>
+        <v>0.17094292150609999</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="25"/>
+        <v>0.80113447284828299</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="25"/>
+        <v>0.10085463621237301</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="25"/>
+        <v>4.1060353955528699E-2</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="25"/>
+        <v>5.6950536983814803E-2</v>
+      </c>
+      <c r="P16">
         <f t="shared" si="23"/>
-        <v>0.40683076923076894</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="24"/>
-        <v>0.82905707849389998</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="24"/>
-        <v>0.17094292150609999</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="24"/>
-        <v>0.80113447284828299</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="24"/>
-        <v>0.10085463621237301</v>
-      </c>
-      <c r="N16">
-        <f t="shared" si="24"/>
-        <v>4.1060353955528699E-2</v>
-      </c>
-      <c r="O16">
-        <f t="shared" si="24"/>
-        <v>5.6950536983814803E-2</v>
-      </c>
-      <c r="P16">
-        <f>P6/$P$2</f>
         <v>1.1793352151568288</v>
       </c>
       <c r="R16">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1.1047345767575303</v>
       </c>
       <c r="S16">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1.6265560165975137</v>
       </c>
     </row>
     <row r="17" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F17">
+        <f t="shared" si="24"/>
+        <v>0.40884615384615403</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="25"/>
+        <v>0.82950268465355503</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="25"/>
+        <v>0.17049731534644499</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="25"/>
+        <v>0.86869614299153297</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="25"/>
+        <v>7.5823142050799597E-2</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="25"/>
+        <v>2.5174035747883301E-2</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="25"/>
+        <v>3.03066792097836E-2</v>
+      </c>
+      <c r="P17">
         <f t="shared" si="23"/>
-        <v>0.40884615384615403</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="24"/>
-        <v>0.82950268465355503</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="24"/>
-        <v>0.17049731534644499</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="24"/>
-        <v>0.86869614299153297</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="24"/>
-        <v>7.5823142050799597E-2</v>
-      </c>
-      <c r="N17">
-        <f t="shared" si="24"/>
-        <v>2.5174035747883301E-2</v>
-      </c>
-      <c r="O17">
-        <f t="shared" si="24"/>
-        <v>3.03066792097836E-2</v>
-      </c>
-      <c r="P17">
-        <f>P7/$P$2</f>
         <v>0.60864247409942807</v>
       </c>
       <c r="R17">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.64421669106881285</v>
       </c>
       <c r="S17">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F18">
+        <f t="shared" si="24"/>
+        <v>0.35338769230769201</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="25"/>
+        <v>0.62105792524658199</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="25"/>
+        <v>0.17552236546115199</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="25"/>
+        <v>0.84268312857528405</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="25"/>
+        <v>7.9546542912120891E-2</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="25"/>
+        <v>3.1249183725000199E-2</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="25"/>
+        <v>4.65211447875944E-2</v>
+      </c>
+      <c r="P18">
         <f t="shared" si="23"/>
-        <v>0.35338769230769201</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="24"/>
-        <v>0.62105792524658199</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="24"/>
-        <v>0.17552236546115199</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="24"/>
-        <v>0.84268312857528405</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="24"/>
-        <v>7.9546542912120891E-2</v>
-      </c>
-      <c r="N18">
-        <f t="shared" si="24"/>
-        <v>3.1249183725000199E-2</v>
-      </c>
-      <c r="O18">
-        <f t="shared" si="24"/>
-        <v>4.65211447875944E-2</v>
-      </c>
-      <c r="P18">
-        <f>P8/$P$2</f>
         <v>1.0010648701303666</v>
       </c>
       <c r="R18">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.99458731381459897</v>
       </c>
       <c r="S18">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.9966101694915287</v>
       </c>
     </row>
     <row r="19" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F19">
+        <f t="shared" si="24"/>
+        <v>0.40688923076923106</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="25"/>
+        <v>0.82595540008745105</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="25"/>
+        <v>0.174044599912549</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="25"/>
+        <v>0.80751518084679996</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="25"/>
+        <v>9.443507588532879E-2</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="25"/>
+        <v>3.9647910223156599E-2</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="25"/>
+        <v>5.8401833044714503E-2</v>
+      </c>
+      <c r="P19">
         <f t="shared" si="23"/>
-        <v>0.40688923076923106</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="24"/>
-        <v>0.82595540008745105</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="24"/>
-        <v>0.174044599912549</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="24"/>
-        <v>0.80751518084679996</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="24"/>
-        <v>9.443507588532879E-2</v>
-      </c>
-      <c r="N19">
-        <f t="shared" si="24"/>
-        <v>3.9647910223156599E-2</v>
-      </c>
-      <c r="O19">
-        <f t="shared" si="24"/>
-        <v>5.8401833044714503E-2</v>
-      </c>
-      <c r="P19">
-        <f>P9/$P$2</f>
         <v>1.1710266996166274</v>
       </c>
       <c r="R19">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1.0784691857107456</v>
       </c>
       <c r="S19">
@@ -9447,39 +9480,39 @@
     </row>
     <row r="20" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F20">
+        <f t="shared" si="24"/>
+        <v>0.40960000000000002</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="25"/>
+        <v>0.77423645959508602</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="25"/>
+        <v>0.22576354040491398</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="25"/>
+        <v>0.80953275240384603</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="25"/>
+        <v>9.3389423076923106E-2</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="25"/>
+        <v>3.9911358173076901E-2</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="25"/>
+        <v>5.7166466346153903E-2</v>
+      </c>
+      <c r="P20">
         <f t="shared" si="23"/>
-        <v>0.40960000000000002</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="24"/>
-        <v>0.77423645959508602</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="24"/>
-        <v>0.22576354040491398</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="24"/>
-        <v>0.80953275240384603</v>
-      </c>
-      <c r="M20">
-        <f t="shared" si="24"/>
-        <v>9.3389423076923106E-2</v>
-      </c>
-      <c r="N20">
-        <f t="shared" si="24"/>
-        <v>3.9911358173076901E-2</v>
-      </c>
-      <c r="O20">
-        <f t="shared" si="24"/>
-        <v>5.7166466346153903E-2</v>
-      </c>
-      <c r="P20">
-        <f>P10/$P$2</f>
         <v>1.146371349591393</v>
       </c>
       <c r="R20">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1.0433604336043341</v>
       </c>
       <c r="S20">
@@ -9498,4 +9531,1772 @@
     <ignoredError sqref="AO2:AO10" formula="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8815D215-4C00-4D69-A4B6-A85223BC21D4}">
+  <dimension ref="A1:AP20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U15" sqref="U15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="21" max="21" width="10.42578125" customWidth="1"/>
+    <col min="22" max="22" width="14.5703125" customWidth="1"/>
+    <col min="39" max="39" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:42" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>68</v>
+      </c>
+      <c r="R1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S1" t="s">
+        <v>58</v>
+      </c>
+      <c r="U1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="V1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="W1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="X1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AK1" s="11"/>
+      <c r="AL1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="AN1" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AP1" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:42" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2">
+        <v>200</v>
+      </c>
+      <c r="D2">
+        <v>325000</v>
+      </c>
+      <c r="E2">
+        <v>114784</v>
+      </c>
+      <c r="F2">
+        <v>35.318153846153798</v>
+      </c>
+      <c r="G2">
+        <v>185042</v>
+      </c>
+      <c r="H2">
+        <v>114784</v>
+      </c>
+      <c r="I2">
+        <v>70258</v>
+      </c>
+      <c r="J2">
+        <v>62.031322618648701</v>
+      </c>
+      <c r="K2">
+        <v>37.968677381351299</v>
+      </c>
+      <c r="L2">
+        <v>85.158210203512695</v>
+      </c>
+      <c r="M2">
+        <v>6.9347644270978499</v>
+      </c>
+      <c r="N2">
+        <v>3.0988639531642002</v>
+      </c>
+      <c r="O2">
+        <v>4.8081614162252597</v>
+      </c>
+      <c r="P2" s="25">
+        <v>0.89152940450751195</v>
+      </c>
+      <c r="Q2">
+        <v>8.6206896551724102E-3</v>
+      </c>
+      <c r="R2">
+        <v>1.8382660338382799</v>
+      </c>
+      <c r="S2">
+        <v>0.17182130584192401</v>
+      </c>
+      <c r="U2" s="2">
+        <v>1</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W2" s="2">
+        <f t="shared" ref="W2:Y10" si="0">C2</f>
+        <v>200</v>
+      </c>
+      <c r="X2" s="3">
+        <f t="shared" si="0"/>
+        <v>325000</v>
+      </c>
+      <c r="Y2" s="3">
+        <f t="shared" si="0"/>
+        <v>114784</v>
+      </c>
+      <c r="Z2" s="5">
+        <f>F12</f>
+        <v>0.35318153846153799</v>
+      </c>
+      <c r="AA2" s="3">
+        <f t="shared" ref="AA2:AC10" si="1">G2</f>
+        <v>185042</v>
+      </c>
+      <c r="AB2" s="3">
+        <f t="shared" si="1"/>
+        <v>114784</v>
+      </c>
+      <c r="AC2" s="3">
+        <f t="shared" si="1"/>
+        <v>70258</v>
+      </c>
+      <c r="AD2" s="4">
+        <f t="shared" ref="AD2:AE10" si="2">J12</f>
+        <v>0.62031322618648699</v>
+      </c>
+      <c r="AE2" s="5">
+        <f t="shared" si="2"/>
+        <v>0.37968677381351301</v>
+      </c>
+      <c r="AF2" s="12"/>
+      <c r="AG2" s="4">
+        <f t="shared" ref="AG2:AJ10" si="3">L12</f>
+        <v>0.85158210203512696</v>
+      </c>
+      <c r="AH2" s="4">
+        <f t="shared" si="3"/>
+        <v>6.9347644270978503E-2</v>
+      </c>
+      <c r="AI2" s="4">
+        <f t="shared" si="3"/>
+        <v>3.0988639531642003E-2</v>
+      </c>
+      <c r="AJ2" s="4">
+        <f t="shared" si="3"/>
+        <v>4.8081614162252595E-2</v>
+      </c>
+      <c r="AK2" s="13"/>
+      <c r="AL2" s="13">
+        <f t="shared" ref="AL2:AL10" si="4">SUM(AH2:AJ2)</f>
+        <v>0.14841789796487309</v>
+      </c>
+      <c r="AM2" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="AN2" s="4">
+        <f t="shared" ref="AN2:AN10" si="5">P12</f>
+        <v>1</v>
+      </c>
+      <c r="AO2" s="4">
+        <f>S12</f>
+        <v>1</v>
+      </c>
+      <c r="AP2" s="4">
+        <f>R12</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>200</v>
+      </c>
+      <c r="D3">
+        <v>325000</v>
+      </c>
+      <c r="E3">
+        <v>114380</v>
+      </c>
+      <c r="F3">
+        <v>35.193846153846202</v>
+      </c>
+      <c r="G3">
+        <v>184363</v>
+      </c>
+      <c r="H3">
+        <v>114380</v>
+      </c>
+      <c r="I3">
+        <v>69983</v>
+      </c>
+      <c r="J3">
+        <v>62.040648069298101</v>
+      </c>
+      <c r="K3">
+        <v>37.959351930701899</v>
+      </c>
+      <c r="L3">
+        <v>85.543801363874806</v>
+      </c>
+      <c r="M3">
+        <v>6.8333624759573404</v>
+      </c>
+      <c r="N3">
+        <v>3.0442385032348298</v>
+      </c>
+      <c r="O3">
+        <v>4.57859765693303</v>
+      </c>
+      <c r="P3" s="25">
+        <v>0.84510827777117303</v>
+      </c>
+      <c r="Q3">
+        <v>8.3892617449664395E-3</v>
+      </c>
+      <c r="R3">
+        <v>1.8018018018018001</v>
+      </c>
+      <c r="S3">
+        <v>0.17006802721088399</v>
+      </c>
+      <c r="U3" s="2">
+        <v>2</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="W3" s="2">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="X3" s="3">
+        <f t="shared" si="0"/>
+        <v>325000</v>
+      </c>
+      <c r="Y3" s="3">
+        <f t="shared" si="0"/>
+        <v>114380</v>
+      </c>
+      <c r="Z3" s="5">
+        <f t="shared" ref="Z3:Z10" si="6">F13</f>
+        <v>0.35193846153846203</v>
+      </c>
+      <c r="AA3" s="3">
+        <f t="shared" si="1"/>
+        <v>184363</v>
+      </c>
+      <c r="AB3" s="3">
+        <f t="shared" si="1"/>
+        <v>114380</v>
+      </c>
+      <c r="AC3" s="3">
+        <f t="shared" si="1"/>
+        <v>69983</v>
+      </c>
+      <c r="AD3" s="4">
+        <f t="shared" si="2"/>
+        <v>0.62040648069298099</v>
+      </c>
+      <c r="AE3" s="5">
+        <f t="shared" si="2"/>
+        <v>0.37959351930701901</v>
+      </c>
+      <c r="AF3" s="12"/>
+      <c r="AG3" s="4">
+        <f t="shared" si="3"/>
+        <v>0.85543801363874805</v>
+      </c>
+      <c r="AH3" s="4">
+        <f t="shared" si="3"/>
+        <v>6.83336247595734E-2</v>
+      </c>
+      <c r="AI3" s="4">
+        <f t="shared" si="3"/>
+        <v>3.0442385032348297E-2</v>
+      </c>
+      <c r="AJ3" s="4">
+        <f t="shared" si="3"/>
+        <v>4.5785976569330297E-2</v>
+      </c>
+      <c r="AK3" s="13"/>
+      <c r="AL3" s="13">
+        <f t="shared" si="4"/>
+        <v>0.144561986361252</v>
+      </c>
+      <c r="AM3" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="AN3" s="4">
+        <f t="shared" si="5"/>
+        <v>0.94793090782913403</v>
+      </c>
+      <c r="AO3" s="4">
+        <f>S13</f>
+        <v>0.98979591836734704</v>
+      </c>
+      <c r="AP3" s="4">
+        <f t="shared" ref="AP3:AP10" si="7">R13</f>
+        <v>0.98016378948136096</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4">
+        <v>200</v>
+      </c>
+      <c r="D4">
+        <v>325000</v>
+      </c>
+      <c r="E4">
+        <v>114931</v>
+      </c>
+      <c r="F4">
+        <v>35.363384615384597</v>
+      </c>
+      <c r="G4">
+        <v>184685</v>
+      </c>
+      <c r="H4">
+        <v>114931</v>
+      </c>
+      <c r="I4">
+        <v>69754</v>
+      </c>
+      <c r="J4">
+        <v>62.230825459566297</v>
+      </c>
+      <c r="K4">
+        <v>37.769174540433703</v>
+      </c>
+      <c r="L4">
+        <v>89.096936422723203</v>
+      </c>
+      <c r="M4">
+        <v>6.2150333678467904</v>
+      </c>
+      <c r="N4">
+        <v>2.0995205819143701</v>
+      </c>
+      <c r="O4">
+        <v>2.5885096275156401</v>
+      </c>
+      <c r="P4" s="25">
+        <v>0.48401514372875198</v>
+      </c>
+      <c r="Q4">
+        <v>4.98338870431894E-3</v>
+      </c>
+      <c r="R4">
+        <v>1.2089810017271201</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="U4" s="2">
+        <v>3</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="W4" s="2">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="X4" s="3">
+        <f t="shared" si="0"/>
+        <v>325000</v>
+      </c>
+      <c r="Y4" s="3">
+        <f t="shared" si="0"/>
+        <v>114931</v>
+      </c>
+      <c r="Z4" s="5">
+        <f t="shared" si="6"/>
+        <v>0.35363384615384597</v>
+      </c>
+      <c r="AA4" s="3">
+        <f t="shared" si="1"/>
+        <v>184685</v>
+      </c>
+      <c r="AB4" s="3">
+        <f t="shared" si="1"/>
+        <v>114931</v>
+      </c>
+      <c r="AC4" s="3">
+        <f t="shared" si="1"/>
+        <v>69754</v>
+      </c>
+      <c r="AD4" s="4">
+        <f t="shared" si="2"/>
+        <v>0.62230825459566297</v>
+      </c>
+      <c r="AE4" s="5">
+        <f t="shared" si="2"/>
+        <v>0.37769174540433703</v>
+      </c>
+      <c r="AF4" s="12"/>
+      <c r="AG4" s="4">
+        <f t="shared" si="3"/>
+        <v>0.89096936422723205</v>
+      </c>
+      <c r="AH4" s="4">
+        <f t="shared" si="3"/>
+        <v>6.2150333678467902E-2</v>
+      </c>
+      <c r="AI4" s="4">
+        <f t="shared" si="3"/>
+        <v>2.09952058191437E-2</v>
+      </c>
+      <c r="AJ4" s="4">
+        <f t="shared" si="3"/>
+        <v>2.5885096275156401E-2</v>
+      </c>
+      <c r="AK4" s="13"/>
+      <c r="AL4" s="13">
+        <f t="shared" si="4"/>
+        <v>0.109030635772768</v>
+      </c>
+      <c r="AM4" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="AN4" s="4">
+        <f t="shared" si="5"/>
+        <v>0.54290429601267709</v>
+      </c>
+      <c r="AO4" s="4">
+        <f t="shared" ref="AO4:AO10" si="8">S14</f>
+        <v>0</v>
+      </c>
+      <c r="AP4" s="4">
+        <f t="shared" si="7"/>
+        <v>0.65767466703542399</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>200</v>
+      </c>
+      <c r="D5">
+        <v>325000</v>
+      </c>
+      <c r="E5">
+        <v>133089</v>
+      </c>
+      <c r="F5">
+        <v>40.950461538461497</v>
+      </c>
+      <c r="G5">
+        <v>171837</v>
+      </c>
+      <c r="H5">
+        <v>142757</v>
+      </c>
+      <c r="I5">
+        <v>29080</v>
+      </c>
+      <c r="J5">
+        <v>83.0769857481218</v>
+      </c>
+      <c r="K5">
+        <v>16.9230142518782</v>
+      </c>
+      <c r="L5">
+        <v>81.499598013359503</v>
+      </c>
+      <c r="M5">
+        <v>8.9751970485915393</v>
+      </c>
+      <c r="N5">
+        <v>3.87409928694332</v>
+      </c>
+      <c r="O5">
+        <v>5.6511056511056497</v>
+      </c>
+      <c r="P5" s="25">
+        <v>0.98375621186715501</v>
+      </c>
+      <c r="Q5">
+        <v>9.5890410958904097E-3</v>
+      </c>
+      <c r="R5">
+        <v>1.92023633677991</v>
+      </c>
+      <c r="S5">
+        <v>0.27322404371584702</v>
+      </c>
+      <c r="U5" s="2">
+        <v>4</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="W5" s="2">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="X5" s="3">
+        <f t="shared" si="0"/>
+        <v>325000</v>
+      </c>
+      <c r="Y5" s="3">
+        <f t="shared" si="0"/>
+        <v>133089</v>
+      </c>
+      <c r="Z5" s="5">
+        <f t="shared" si="6"/>
+        <v>0.40950461538461497</v>
+      </c>
+      <c r="AA5" s="3">
+        <f t="shared" si="1"/>
+        <v>171837</v>
+      </c>
+      <c r="AB5" s="3">
+        <f t="shared" si="1"/>
+        <v>142757</v>
+      </c>
+      <c r="AC5" s="3">
+        <f t="shared" si="1"/>
+        <v>29080</v>
+      </c>
+      <c r="AD5" s="4">
+        <f t="shared" si="2"/>
+        <v>0.83076985748121801</v>
+      </c>
+      <c r="AE5" s="5">
+        <f t="shared" si="2"/>
+        <v>0.16923014251878199</v>
+      </c>
+      <c r="AF5" s="12"/>
+      <c r="AG5" s="4">
+        <f t="shared" si="3"/>
+        <v>0.81499598013359498</v>
+      </c>
+      <c r="AH5" s="4">
+        <f t="shared" si="3"/>
+        <v>8.9751970485915392E-2</v>
+      </c>
+      <c r="AI5" s="4">
+        <f t="shared" si="3"/>
+        <v>3.8740992869433201E-2</v>
+      </c>
+      <c r="AJ5" s="4">
+        <f t="shared" si="3"/>
+        <v>5.65110565110565E-2</v>
+      </c>
+      <c r="AK5" s="13"/>
+      <c r="AL5" s="13">
+        <f t="shared" si="4"/>
+        <v>0.18500401986640511</v>
+      </c>
+      <c r="AM5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AN5" s="4">
+        <f t="shared" si="5"/>
+        <v>1.1034478581338434</v>
+      </c>
+      <c r="AO5" s="4">
+        <f t="shared" si="8"/>
+        <v>1.5901639344262333</v>
+      </c>
+      <c r="AP5" s="4">
+        <f t="shared" si="7"/>
+        <v>1.0445910991296929</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6">
+        <v>200</v>
+      </c>
+      <c r="D6">
+        <v>325000</v>
+      </c>
+      <c r="E6">
+        <v>132479</v>
+      </c>
+      <c r="F6">
+        <v>40.762769230769202</v>
+      </c>
+      <c r="G6">
+        <v>171348</v>
+      </c>
+      <c r="H6">
+        <v>142138</v>
+      </c>
+      <c r="I6">
+        <v>29210</v>
+      </c>
+      <c r="J6">
+        <v>82.952821159278201</v>
+      </c>
+      <c r="K6">
+        <v>17.047178840721799</v>
+      </c>
+      <c r="L6">
+        <v>82.7466994768982</v>
+      </c>
+      <c r="M6">
+        <v>8.4307701597989109</v>
+      </c>
+      <c r="N6">
+        <v>3.6315189577216</v>
+      </c>
+      <c r="O6">
+        <v>5.1910114055812597</v>
+      </c>
+      <c r="P6" s="25">
+        <v>0.89782085063755102</v>
+      </c>
+      <c r="Q6">
+        <v>8.5470085470085496E-3</v>
+      </c>
+      <c r="R6">
+        <v>1.7595307917888601</v>
+      </c>
+      <c r="S6">
+        <v>0.26845637583892601</v>
+      </c>
+      <c r="U6" s="2">
+        <v>5</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="W6" s="2">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="X6" s="3">
+        <f t="shared" si="0"/>
+        <v>325000</v>
+      </c>
+      <c r="Y6" s="3">
+        <f t="shared" si="0"/>
+        <v>132479</v>
+      </c>
+      <c r="Z6" s="5">
+        <f t="shared" si="6"/>
+        <v>0.40762769230769202</v>
+      </c>
+      <c r="AA6" s="3">
+        <f t="shared" si="1"/>
+        <v>171348</v>
+      </c>
+      <c r="AB6" s="3">
+        <f t="shared" si="1"/>
+        <v>142138</v>
+      </c>
+      <c r="AC6" s="3">
+        <f t="shared" si="1"/>
+        <v>29210</v>
+      </c>
+      <c r="AD6" s="4">
+        <f t="shared" si="2"/>
+        <v>0.82952821159278201</v>
+      </c>
+      <c r="AE6" s="5">
+        <f t="shared" si="2"/>
+        <v>0.17047178840721799</v>
+      </c>
+      <c r="AF6" s="12"/>
+      <c r="AG6" s="4">
+        <f t="shared" si="3"/>
+        <v>0.827466994768982</v>
+      </c>
+      <c r="AH6" s="4">
+        <f t="shared" si="3"/>
+        <v>8.4307701597989115E-2</v>
+      </c>
+      <c r="AI6" s="4">
+        <f t="shared" si="3"/>
+        <v>3.6315189577216002E-2</v>
+      </c>
+      <c r="AJ6" s="4">
+        <f t="shared" si="3"/>
+        <v>5.1910114055812598E-2</v>
+      </c>
+      <c r="AK6" s="13"/>
+      <c r="AL6" s="13">
+        <f t="shared" si="4"/>
+        <v>0.17253300523101772</v>
+      </c>
+      <c r="AM6" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="AN6" s="4">
+        <f t="shared" si="5"/>
+        <v>1.0070569137688896</v>
+      </c>
+      <c r="AO6" s="4">
+        <f t="shared" si="8"/>
+        <v>1.5624161073825529</v>
+      </c>
+      <c r="AP6" s="4">
+        <f t="shared" si="7"/>
+        <v>0.9571687445668452</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>200</v>
+      </c>
+      <c r="D7">
+        <v>325000</v>
+      </c>
+      <c r="E7">
+        <v>132381</v>
+      </c>
+      <c r="F7">
+        <v>40.7326153846154</v>
+      </c>
+      <c r="G7">
+        <v>171328</v>
+      </c>
+      <c r="H7">
+        <v>142059</v>
+      </c>
+      <c r="I7">
+        <v>29269</v>
+      </c>
+      <c r="J7">
+        <v>82.916394284646998</v>
+      </c>
+      <c r="K7">
+        <v>17.083605715352999</v>
+      </c>
+      <c r="L7">
+        <v>87.081983064034901</v>
+      </c>
+      <c r="M7">
+        <v>7.3862563358790201</v>
+      </c>
+      <c r="N7">
+        <v>2.5011142082323001</v>
+      </c>
+      <c r="O7">
+        <v>3.03064639185382</v>
+      </c>
+      <c r="P7" s="25">
+        <v>0.52371221772742604</v>
+      </c>
+      <c r="Q7">
+        <v>5.2219321148825101E-3</v>
+      </c>
+      <c r="R7">
+        <v>1.16279069767442</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="U7" s="2">
+        <v>6</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="W7" s="2">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="X7" s="3">
+        <f t="shared" si="0"/>
+        <v>325000</v>
+      </c>
+      <c r="Y7" s="3">
+        <f t="shared" si="0"/>
+        <v>132381</v>
+      </c>
+      <c r="Z7" s="5">
+        <f t="shared" si="6"/>
+        <v>0.407326153846154</v>
+      </c>
+      <c r="AA7" s="3">
+        <f t="shared" si="1"/>
+        <v>171328</v>
+      </c>
+      <c r="AB7" s="3">
+        <f t="shared" si="1"/>
+        <v>142059</v>
+      </c>
+      <c r="AC7" s="3">
+        <f t="shared" si="1"/>
+        <v>29269</v>
+      </c>
+      <c r="AD7" s="4">
+        <f t="shared" si="2"/>
+        <v>0.82916394284646999</v>
+      </c>
+      <c r="AE7" s="5">
+        <f t="shared" si="2"/>
+        <v>0.17083605715352998</v>
+      </c>
+      <c r="AF7" s="12"/>
+      <c r="AG7" s="4">
+        <f t="shared" si="3"/>
+        <v>0.87081983064034896</v>
+      </c>
+      <c r="AH7" s="4">
+        <f t="shared" si="3"/>
+        <v>7.3862563358790198E-2</v>
+      </c>
+      <c r="AI7" s="4">
+        <f t="shared" si="3"/>
+        <v>2.5011142082323003E-2</v>
+      </c>
+      <c r="AJ7" s="4">
+        <f t="shared" si="3"/>
+        <v>3.0306463918538199E-2</v>
+      </c>
+      <c r="AK7" s="13"/>
+      <c r="AL7" s="13">
+        <f t="shared" si="4"/>
+        <v>0.1291801693596514</v>
+      </c>
+      <c r="AM7" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AN7" s="4">
+        <f t="shared" si="5"/>
+        <v>0.58743123342827808</v>
+      </c>
+      <c r="AO7" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AP7" s="4">
+        <f t="shared" si="7"/>
+        <v>0.63254756181646099</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8">
+        <v>200</v>
+      </c>
+      <c r="D8">
+        <v>325000</v>
+      </c>
+      <c r="E8">
+        <v>114305</v>
+      </c>
+      <c r="F8">
+        <v>35.170769230769203</v>
+      </c>
+      <c r="G8">
+        <v>184508</v>
+      </c>
+      <c r="H8">
+        <v>114305</v>
+      </c>
+      <c r="I8">
+        <v>35794</v>
+      </c>
+      <c r="J8">
+        <v>61.951243306523303</v>
+      </c>
+      <c r="K8">
+        <v>19.3997008259804</v>
+      </c>
+      <c r="L8">
+        <v>84.092559380604499</v>
+      </c>
+      <c r="M8">
+        <v>7.8789204321770701</v>
+      </c>
+      <c r="N8">
+        <v>3.3646822098770799</v>
+      </c>
+      <c r="O8">
+        <v>4.6638379773413199</v>
+      </c>
+      <c r="P8" s="25">
+        <v>0.86767578512388599</v>
+      </c>
+      <c r="Q8">
+        <v>8.5034013605442202E-3</v>
+      </c>
+      <c r="R8">
+        <v>1.8518518518518501</v>
+      </c>
+      <c r="S8">
+        <v>0.17123287671232901</v>
+      </c>
+      <c r="U8" s="2">
+        <v>7</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="W8" s="2">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="X8" s="3">
+        <f t="shared" si="0"/>
+        <v>325000</v>
+      </c>
+      <c r="Y8" s="3">
+        <f t="shared" si="0"/>
+        <v>114305</v>
+      </c>
+      <c r="Z8" s="5">
+        <f t="shared" si="6"/>
+        <v>0.35170769230769205</v>
+      </c>
+      <c r="AA8" s="3">
+        <f t="shared" si="1"/>
+        <v>184508</v>
+      </c>
+      <c r="AB8" s="3">
+        <f t="shared" si="1"/>
+        <v>114305</v>
+      </c>
+      <c r="AC8" s="3">
+        <f t="shared" si="1"/>
+        <v>35794</v>
+      </c>
+      <c r="AD8" s="4">
+        <f t="shared" si="2"/>
+        <v>0.61951243306523307</v>
+      </c>
+      <c r="AE8" s="5">
+        <f t="shared" si="2"/>
+        <v>0.19399700825980401</v>
+      </c>
+      <c r="AF8" s="12"/>
+      <c r="AG8" s="4">
+        <f t="shared" si="3"/>
+        <v>0.84092559380604504</v>
+      </c>
+      <c r="AH8" s="4">
+        <f t="shared" si="3"/>
+        <v>7.8789204321770695E-2</v>
+      </c>
+      <c r="AI8" s="4">
+        <f t="shared" si="3"/>
+        <v>3.3646822098770797E-2</v>
+      </c>
+      <c r="AJ8" s="4">
+        <f t="shared" si="3"/>
+        <v>4.6638379773413202E-2</v>
+      </c>
+      <c r="AK8" s="13"/>
+      <c r="AL8" s="13">
+        <f>SUM(AH8:AJ8)</f>
+        <v>0.15907440619395469</v>
+      </c>
+      <c r="AM8" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="AN8" s="4">
+        <f t="shared" si="5"/>
+        <v>0.97324415856277569</v>
+      </c>
+      <c r="AO8" s="4">
+        <f t="shared" si="8"/>
+        <v>0.99657534246575707</v>
+      </c>
+      <c r="AP8" s="4">
+        <f t="shared" si="7"/>
+        <v>1.0073905614113987</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9">
+        <v>200</v>
+      </c>
+      <c r="D9">
+        <v>325000</v>
+      </c>
+      <c r="E9">
+        <v>132217</v>
+      </c>
+      <c r="F9">
+        <v>40.682153846153803</v>
+      </c>
+      <c r="G9">
+        <v>171484</v>
+      </c>
+      <c r="H9">
+        <v>141579</v>
+      </c>
+      <c r="I9">
+        <v>29905</v>
+      </c>
+      <c r="J9">
+        <v>82.561055258799698</v>
+      </c>
+      <c r="K9">
+        <v>17.438944741200299</v>
+      </c>
+      <c r="L9">
+        <v>82.3237556441305</v>
+      </c>
+      <c r="M9">
+        <v>8.4951254377273706</v>
+      </c>
+      <c r="N9">
+        <v>3.7090540550761202</v>
+      </c>
+      <c r="O9">
+        <v>5.47206486306602</v>
+      </c>
+      <c r="P9" s="25">
+        <v>0.93290561748767598</v>
+      </c>
+      <c r="Q9">
+        <v>8.7591240875912399E-3</v>
+      </c>
+      <c r="R9">
+        <v>1.8492176386913199</v>
+      </c>
+      <c r="S9">
+        <v>0.27210884353741499</v>
+      </c>
+      <c r="U9" s="2">
+        <v>8</v>
+      </c>
+      <c r="V9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="W9" s="2">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="X9" s="3">
+        <f t="shared" si="0"/>
+        <v>325000</v>
+      </c>
+      <c r="Y9" s="3">
+        <f t="shared" si="0"/>
+        <v>132217</v>
+      </c>
+      <c r="Z9" s="5">
+        <f t="shared" si="6"/>
+        <v>0.40682153846153801</v>
+      </c>
+      <c r="AA9" s="3">
+        <f t="shared" si="1"/>
+        <v>171484</v>
+      </c>
+      <c r="AB9" s="3">
+        <f t="shared" si="1"/>
+        <v>141579</v>
+      </c>
+      <c r="AC9" s="3">
+        <f t="shared" si="1"/>
+        <v>29905</v>
+      </c>
+      <c r="AD9" s="4">
+        <f t="shared" si="2"/>
+        <v>0.82561055258799698</v>
+      </c>
+      <c r="AE9" s="5">
+        <f t="shared" si="2"/>
+        <v>0.17438944741200299</v>
+      </c>
+      <c r="AF9" s="12"/>
+      <c r="AG9" s="4">
+        <f t="shared" si="3"/>
+        <v>0.82323755644130503</v>
+      </c>
+      <c r="AH9" s="4">
+        <f t="shared" si="3"/>
+        <v>8.4951254377273702E-2</v>
+      </c>
+      <c r="AI9" s="4">
+        <f t="shared" si="3"/>
+        <v>3.7090540550761199E-2</v>
+      </c>
+      <c r="AJ9" s="4">
+        <f t="shared" si="3"/>
+        <v>5.4720648630660201E-2</v>
+      </c>
+      <c r="AK9" s="13"/>
+      <c r="AL9" s="13">
+        <f t="shared" si="4"/>
+        <v>0.17676244355869511</v>
+      </c>
+      <c r="AM9" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="AN9" s="4">
+        <f t="shared" si="5"/>
+        <v>1.046410373870978</v>
+      </c>
+      <c r="AO9" s="4">
+        <f t="shared" si="8"/>
+        <v>1.5836734693877588</v>
+      </c>
+      <c r="AP9" s="4">
+        <f t="shared" si="7"/>
+        <v>1.0059575734150803</v>
+      </c>
+    </row>
+    <row r="10" spans="1:42" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10">
+        <v>200</v>
+      </c>
+      <c r="D10">
+        <v>325000</v>
+      </c>
+      <c r="E10">
+        <v>133362</v>
+      </c>
+      <c r="F10">
+        <v>41.0344615384615</v>
+      </c>
+      <c r="G10">
+        <v>184508</v>
+      </c>
+      <c r="H10">
+        <v>143333</v>
+      </c>
+      <c r="I10">
+        <v>41175</v>
+      </c>
+      <c r="J10">
+        <v>77.683894465280602</v>
+      </c>
+      <c r="K10">
+        <v>22.316105534719402</v>
+      </c>
+      <c r="L10">
+        <v>82.831691186394906</v>
+      </c>
+      <c r="M10">
+        <v>8.2197327574571499</v>
+      </c>
+      <c r="N10">
+        <v>3.5864789070349898</v>
+      </c>
+      <c r="O10">
+        <v>5.3620971491129401</v>
+      </c>
+      <c r="P10" s="25">
+        <v>0.91975709990487198</v>
+      </c>
+      <c r="Q10">
+        <v>8.5959885386819503E-3</v>
+      </c>
+      <c r="R10">
+        <v>1.8413597733711</v>
+      </c>
+      <c r="S10">
+        <v>0.26737967914438499</v>
+      </c>
+      <c r="U10" s="2">
+        <v>9</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="W10" s="2">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="X10" s="3">
+        <f t="shared" si="0"/>
+        <v>325000</v>
+      </c>
+      <c r="Y10" s="3">
+        <f t="shared" si="0"/>
+        <v>133362</v>
+      </c>
+      <c r="Z10" s="5">
+        <f t="shared" si="6"/>
+        <v>0.41034461538461497</v>
+      </c>
+      <c r="AA10" s="3">
+        <f t="shared" si="1"/>
+        <v>184508</v>
+      </c>
+      <c r="AB10" s="3">
+        <f t="shared" si="1"/>
+        <v>143333</v>
+      </c>
+      <c r="AC10" s="3">
+        <f t="shared" si="1"/>
+        <v>41175</v>
+      </c>
+      <c r="AD10" s="4">
+        <f t="shared" si="2"/>
+        <v>0.77683894465280601</v>
+      </c>
+      <c r="AE10" s="5">
+        <f t="shared" si="2"/>
+        <v>0.22316105534719402</v>
+      </c>
+      <c r="AG10" s="4">
+        <f t="shared" si="3"/>
+        <v>0.82831691186394907</v>
+      </c>
+      <c r="AH10" s="4">
+        <f t="shared" si="3"/>
+        <v>8.2197327574571502E-2</v>
+      </c>
+      <c r="AI10" s="4">
+        <f t="shared" si="3"/>
+        <v>3.5864789070349901E-2</v>
+      </c>
+      <c r="AJ10" s="4">
+        <f t="shared" si="3"/>
+        <v>5.3620971491129404E-2</v>
+      </c>
+      <c r="AL10" s="13">
+        <f t="shared" si="4"/>
+        <v>0.17168308813605082</v>
+      </c>
+      <c r="AM10" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="AN10" s="4">
+        <f t="shared" si="5"/>
+        <v>1.0316621025113055</v>
+      </c>
+      <c r="AO10" s="4">
+        <f t="shared" si="8"/>
+        <v>1.5561497326203242</v>
+      </c>
+      <c r="AP10" s="4">
+        <f t="shared" si="7"/>
+        <v>1.0016829661626072</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>100</v>
+      </c>
+      <c r="F12">
+        <f>F2/$A$12</f>
+        <v>0.35318153846153799</v>
+      </c>
+      <c r="J12">
+        <f>J2/$A$12</f>
+        <v>0.62031322618648699</v>
+      </c>
+      <c r="K12">
+        <f>K2/$A$12</f>
+        <v>0.37968677381351301</v>
+      </c>
+      <c r="L12">
+        <f t="shared" ref="L12:O12" si="9">L2/$A$12</f>
+        <v>0.85158210203512696</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="9"/>
+        <v>6.9347644270978503E-2</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="9"/>
+        <v>3.0988639531642003E-2</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="9"/>
+        <v>4.8081614162252595E-2</v>
+      </c>
+      <c r="P12">
+        <f t="shared" ref="P12:P20" si="10">P2/$P$2</f>
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <f>R2/$R$2</f>
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <f>S2/$S$2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <f t="shared" ref="F13:F20" si="11">F3/$A$12</f>
+        <v>0.35193846153846203</v>
+      </c>
+      <c r="J13">
+        <f t="shared" ref="J13:O20" si="12">J3/$A$12</f>
+        <v>0.62040648069298099</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="12"/>
+        <v>0.37959351930701901</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="12"/>
+        <v>0.85543801363874805</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="12"/>
+        <v>6.83336247595734E-2</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="12"/>
+        <v>3.0442385032348297E-2</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="12"/>
+        <v>4.5785976569330297E-2</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="10"/>
+        <v>0.94793090782913403</v>
+      </c>
+      <c r="R13">
+        <f t="shared" ref="R13:R20" si="13">R3/$R$2</f>
+        <v>0.98016378948136096</v>
+      </c>
+      <c r="S13">
+        <f t="shared" ref="S13:S18" si="14">S3/$S$2</f>
+        <v>0.98979591836734704</v>
+      </c>
+    </row>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <f t="shared" si="11"/>
+        <v>0.35363384615384597</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="12"/>
+        <v>0.62230825459566297</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="12"/>
+        <v>0.37769174540433703</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="12"/>
+        <v>0.89096936422723205</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="12"/>
+        <v>6.2150333678467902E-2</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="12"/>
+        <v>2.09952058191437E-2</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="12"/>
+        <v>2.5885096275156401E-2</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="10"/>
+        <v>0.54290429601267709</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="13"/>
+        <v>0.65767466703542399</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <f t="shared" si="11"/>
+        <v>0.40950461538461497</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="12"/>
+        <v>0.83076985748121801</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="12"/>
+        <v>0.16923014251878199</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="12"/>
+        <v>0.81499598013359498</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="12"/>
+        <v>8.9751970485915392E-2</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="12"/>
+        <v>3.8740992869433201E-2</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="12"/>
+        <v>5.65110565110565E-2</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="10"/>
+        <v>1.1034478581338434</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="13"/>
+        <v>1.0445910991296929</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="14"/>
+        <v>1.5901639344262333</v>
+      </c>
+    </row>
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <f t="shared" si="11"/>
+        <v>0.40762769230769202</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="12"/>
+        <v>0.82952821159278201</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="12"/>
+        <v>0.17047178840721799</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="12"/>
+        <v>0.827466994768982</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="12"/>
+        <v>8.4307701597989115E-2</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="12"/>
+        <v>3.6315189577216002E-2</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="12"/>
+        <v>5.1910114055812598E-2</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="10"/>
+        <v>1.0070569137688896</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="13"/>
+        <v>0.9571687445668452</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="14"/>
+        <v>1.5624161073825529</v>
+      </c>
+    </row>
+    <row r="17" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <f t="shared" si="11"/>
+        <v>0.407326153846154</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="12"/>
+        <v>0.82916394284646999</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="12"/>
+        <v>0.17083605715352998</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="12"/>
+        <v>0.87081983064034896</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="12"/>
+        <v>7.3862563358790198E-2</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="12"/>
+        <v>2.5011142082323003E-2</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="12"/>
+        <v>3.0306463918538199E-2</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="10"/>
+        <v>0.58743123342827808</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="13"/>
+        <v>0.63254756181646099</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <f t="shared" si="11"/>
+        <v>0.35170769230769205</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="12"/>
+        <v>0.61951243306523307</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="12"/>
+        <v>0.19399700825980401</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="12"/>
+        <v>0.84092559380604504</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="12"/>
+        <v>7.8789204321770695E-2</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="12"/>
+        <v>3.3646822098770797E-2</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="12"/>
+        <v>4.6638379773413202E-2</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="10"/>
+        <v>0.97324415856277569</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="13"/>
+        <v>1.0073905614113987</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="14"/>
+        <v>0.99657534246575707</v>
+      </c>
+    </row>
+    <row r="19" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <f t="shared" si="11"/>
+        <v>0.40682153846153801</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="12"/>
+        <v>0.82561055258799698</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="12"/>
+        <v>0.17438944741200299</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="12"/>
+        <v>0.82323755644130503</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="12"/>
+        <v>8.4951254377273702E-2</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="12"/>
+        <v>3.7090540550761199E-2</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="12"/>
+        <v>5.4720648630660201E-2</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="10"/>
+        <v>1.046410373870978</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="13"/>
+        <v>1.0059575734150803</v>
+      </c>
+      <c r="S19">
+        <f>S9/$S$2</f>
+        <v>1.5836734693877588</v>
+      </c>
+    </row>
+    <row r="20" spans="6:19" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <f t="shared" si="11"/>
+        <v>0.41034461538461497</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="12"/>
+        <v>0.77683894465280601</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="12"/>
+        <v>0.22316105534719402</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="12"/>
+        <v>0.82831691186394907</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="12"/>
+        <v>8.2197327574571502E-2</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="12"/>
+        <v>3.5864789070349901E-2</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="12"/>
+        <v>5.3620971491129404E-2</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="10"/>
+        <v>1.0316621025113055</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="13"/>
+        <v>1.0016829661626072</v>
+      </c>
+      <c r="S20">
+        <f>S10/$S$2</f>
+        <v>1.5561497326203242</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:S1" xr:uid="{00000000-0009-0000-0000-000004000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S10">
+      <sortCondition ref="B1"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>